<commit_message>
added bunch of testing
</commit_message>
<xml_diff>
--- a/history/9709_12_2024_MayJune_Mathematics_qp.xlsx
+++ b/history/9709_12_2024_MayJune_Mathematics_qp.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,11 +476,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1(a)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -497,36 +497,283 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Too smart a monkey to receive such a score</t>
+          <t>Strong on transformations and composition (Q2), trigonometric manipulation and solving (Q3), inverse functions and composite functions (Q4), geometric and arithmetic progressions (Q5b), differentiation and integration including use of limits (Q6, Q9b, Q10a), and circle geometry with tangents (Q7). Working generally clear and follows required methods.</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Too dumb a human to perform so poor</t>
+          <t>Occasional algebraic/numerical accuracy slips leading to wrong final values (Q1 binomial coefficient, Q5a sum of AP, Q8b perimeter equation solved inaccurately, Q10b perpendicular bisector). Some inconsistency in deciding increasing/decreasing intervals (Q9a). Perpendicular bisector method and presentation of gradients/midpoint need more care. Ensure final answers are clearly stated and checked for reasonableness; show key intermediate values explicitly where required by the mark scheme.</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="N2" t="n">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>U</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1(b)</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3(a)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3(b)</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>4(a)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>4(b)</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>4(c)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5(a)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5(b)(i)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5(b)(ii)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6(a)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6(b)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>7(a)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>7(b)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>8(a)(i)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>8(a)(ii)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>8(b)</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>9(a)</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>9(b)</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10(a)</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>10(b)</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
         <v>6</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C22" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>